<commit_message>
Sanity check code for calculating ROE by CAPM method
It fixes #45
It involves doing sanity testing for #36, #21 and #8.
</commit_message>
<xml_diff>
--- a/excelSheets/WACC.xlsx
+++ b/excelSheets/WACC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="497">
   <si>
     <t xml:space="preserve">Column1</t>
   </si>
@@ -1535,7 +1535,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mmm"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
@@ -1545,8 +1545,9 @@
     <numFmt numFmtId="170" formatCode="0.00%"/>
     <numFmt numFmtId="171" formatCode="0.0%"/>
     <numFmt numFmtId="172" formatCode="d\ mmm\ yy"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="0.00000%"/>
+    <numFmt numFmtId="173" formatCode="General"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="175" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1704,7 +1705,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1773,7 +1774,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1882,9 +1891,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>218160</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1894,7 +1903,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3592080" y="1285920"/>
-          <a:ext cx="4479480" cy="893880"/>
+          <a:ext cx="4479120" cy="893520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3148,8 +3157,8 @@
   </sheetPr>
   <dimension ref="A1:L252"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3250,7 +3259,7 @@
       <c r="J4" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="K4" s="15" t="n">
+      <c r="K4" s="16" t="n">
         <f aca="false">_xlfn.COVARIANCE.P(C4:C252,H4:H252)/_xlfn.VAR.P(C4:C252)</f>
         <v>1.28818482776349</v>
       </c>
@@ -3284,7 +3293,7 @@
       <c r="J5" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="K5" s="16" t="n">
+      <c r="K5" s="17" t="n">
         <f aca="false">AVERAGE(C4:C252)</f>
         <v>0.000703334461799799</v>
       </c>
@@ -3352,9 +3361,13 @@
       <c r="J7" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="K7" s="16" t="n">
+      <c r="K7" s="17" t="n">
         <f aca="false">AVERAGE(H4:H252)</f>
         <v>0.000768719287199422</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">_xlfn.FORMULATEXT(K7)</f>
+        <v>=AVERAGE(H4:H252)</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,6 +3398,10 @@
       <c r="K8" s="8" t="n">
         <f aca="false">((1+K7)^365)-1</f>
         <v>0.323758117955684</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">_xlfn.FORMULATEXT(K8)</f>
+        <v>=((1+K7)^365)-1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9024,8 +9041,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9034,6 +9051,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9128,18 +9146,18 @@
         <v>0.292562706487598</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="B9" s="17" t="n">
+      <c r="B9" s="18" t="n">
         <f aca="false">B7/B5</f>
         <v>0.0759872582632379</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="19" t="n">
         <f aca="false">'Risk Free Return'!D3</f>
         <v>0.0376</v>
       </c>
@@ -9153,17 +9171,15 @@
       </c>
       <c r="F11" s="8" t="n">
         <f aca="false">F9+F7*(F8-F9)</f>
-        <v>0.590869073078087</v>
+        <v>0.590869073078088</v>
       </c>
       <c r="G11" s="0" t="str">
         <f aca="false">_xlfn.FORMULATEXT(F11)</f>
         <v>=F9+F7*(F8-F9)</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="0" t="s">
-        <v>409</v>
-      </c>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -9232,7 +9248,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="11" t="n">
         <f aca="false">F17*F11+B17*B9*(1-0.3)</f>
-        <v>0.248477866149449</v>
+        <v>0.24847786614945</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.FORMULATEXT(B20)</f>
@@ -9269,72 +9285,72 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="B3" s="19" t="n">
+      <c r="B3" s="21" t="n">
         <v>2007</v>
       </c>
-      <c r="C3" s="19" t="n">
+      <c r="C3" s="21" t="n">
         <f aca="false">B3+1</f>
         <v>2008</v>
       </c>
-      <c r="D3" s="19" t="n">
+      <c r="D3" s="21" t="n">
         <f aca="false">C3+1</f>
         <v>2009</v>
       </c>
-      <c r="E3" s="19" t="n">
+      <c r="E3" s="21" t="n">
         <f aca="false">D3+1</f>
         <v>2010</v>
       </c>
-      <c r="F3" s="19" t="n">
+      <c r="F3" s="21" t="n">
         <f aca="false">E3+1</f>
         <v>2011</v>
       </c>
-      <c r="G3" s="19" t="n">
+      <c r="G3" s="21" t="n">
         <f aca="false">F3+1</f>
         <v>2012</v>
       </c>
-      <c r="H3" s="19" t="n">
+      <c r="H3" s="21" t="n">
         <f aca="false">G3+1</f>
         <v>2013</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="21" t="n">
         <f aca="false">H3+1</f>
         <v>2014</v>
       </c>
-      <c r="J3" s="19" t="n">
+      <c r="J3" s="21" t="n">
         <f aca="false">I3+1</f>
         <v>2015</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="K3" s="21" t="n">
         <f aca="false">J3+1</f>
         <v>2016</v>
       </c>
-      <c r="L3" s="19" t="n">
+      <c r="L3" s="21" t="n">
         <f aca="false">K3+1</f>
         <v>2017</v>
       </c>
-      <c r="M3" s="19" t="n">
+      <c r="M3" s="21" t="n">
         <f aca="false">L3+1</f>
         <v>2018</v>
       </c>
-      <c r="N3" s="19" t="n">
+      <c r="N3" s="21" t="n">
         <f aca="false">M3+1</f>
         <v>2019</v>
       </c>
-      <c r="O3" s="19" t="n">
+      <c r="O3" s="21" t="n">
         <f aca="false">N3+1</f>
         <v>2020</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>482</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -9381,7 +9397,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>483</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -9390,120 +9406,120 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="18" t="n">
+      <c r="D7" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="18" t="n">
+      <c r="F7" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="18" t="n">
+      <c r="G7" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="18" t="n">
+      <c r="H7" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="I7" s="18" t="n">
+      <c r="I7" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J7" s="18" t="n">
+      <c r="J7" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="K7" s="18" t="n">
+      <c r="K7" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="L7" s="18" t="n">
+      <c r="L7" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="M7" s="18" t="n">
+      <c r="M7" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="N7" s="18" t="n">
+      <c r="N7" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="O7" s="18" t="n">
+      <c r="O7" s="20" t="n">
         <v>14</v>
       </c>
-      <c r="P7" s="18" t="n">
+      <c r="P7" s="20" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="B8" s="19" t="n">
+      <c r="B8" s="21" t="n">
         <v>2021</v>
       </c>
-      <c r="C8" s="19" t="n">
+      <c r="C8" s="21" t="n">
         <f aca="false">B8+1</f>
         <v>2022</v>
       </c>
-      <c r="D8" s="19" t="n">
+      <c r="D8" s="21" t="n">
         <f aca="false">C8+1</f>
         <v>2023</v>
       </c>
-      <c r="E8" s="19" t="n">
+      <c r="E8" s="21" t="n">
         <f aca="false">D8+1</f>
         <v>2024</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="F8" s="21" t="n">
         <f aca="false">E8+1</f>
         <v>2025</v>
       </c>
-      <c r="G8" s="19" t="n">
+      <c r="G8" s="21" t="n">
         <f aca="false">F8+1</f>
         <v>2026</v>
       </c>
-      <c r="H8" s="19" t="n">
+      <c r="H8" s="21" t="n">
         <f aca="false">G8+1</f>
         <v>2027</v>
       </c>
-      <c r="I8" s="19" t="n">
+      <c r="I8" s="21" t="n">
         <f aca="false">H8+1</f>
         <v>2028</v>
       </c>
-      <c r="J8" s="19" t="n">
+      <c r="J8" s="21" t="n">
         <f aca="false">I8+1</f>
         <v>2029</v>
       </c>
-      <c r="K8" s="19" t="n">
+      <c r="K8" s="21" t="n">
         <f aca="false">J8+1</f>
         <v>2030</v>
       </c>
-      <c r="L8" s="19" t="n">
+      <c r="L8" s="21" t="n">
         <f aca="false">K8+1</f>
         <v>2031</v>
       </c>
-      <c r="M8" s="19" t="n">
+      <c r="M8" s="21" t="n">
         <f aca="false">L8+1</f>
         <v>2032</v>
       </c>
-      <c r="N8" s="19" t="n">
+      <c r="N8" s="21" t="n">
         <f aca="false">M8+1</f>
         <v>2033</v>
       </c>
-      <c r="O8" s="19" t="n">
+      <c r="O8" s="21" t="n">
         <f aca="false">N8+1</f>
         <v>2034</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="21" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>482</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -9572,7 +9588,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="21" t="s">
         <v>486</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -9637,7 +9653,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="20" t="s">
         <v>487</v>
       </c>
       <c r="B12" s="11" t="n">
@@ -9645,7 +9661,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="20" t="s">
         <v>488</v>
       </c>
       <c r="B13" s="12" t="n">
@@ -9653,7 +9669,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>489</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -9666,7 +9682,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>490</v>
       </c>
       <c r="B16" s="0" t="str">
@@ -9679,7 +9695,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="20" t="s">
         <v>459</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -9692,7 +9708,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="20" t="s">
         <v>491</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -9705,7 +9721,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="20" t="s">
         <v>492</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -9713,7 +9729,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="22" t="s">
         <v>493</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -9726,7 +9742,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="20" t="s">
         <v>494</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -9734,7 +9750,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>495</v>
       </c>
       <c r="B22" s="8" t="n">
@@ -9747,7 +9763,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="20" t="s">
         <v>480</v>
       </c>
       <c r="B23" s="12" t="n">
@@ -9756,7 +9772,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>496</v>
       </c>
       <c r="B24" s="0" t="str">
@@ -11164,7 +11180,7 @@
   </sheetPr>
   <dimension ref="A2:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -11525,7 +11541,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B35" r:id="rId1" display="https://www.youtube.com/watch?v=nhJaAC0BUVQ"/>
+    <hyperlink ref="B35" r:id="rId1" display="Source : https://www.youtube.com/watch?v=nhJaAC0BUVQ"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -11917,10 +11933,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E246"/>
+  <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11962,6 +11978,9 @@
       <c r="D3" s="8" t="n">
         <v>0.0376</v>
       </c>
+      <c r="F3" s="11" t="n">
+        <v>0.0375</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="n">
@@ -11977,6 +11996,10 @@
       <c r="E4" s="0" t="str">
         <f aca="false">_xlfn.FORMULATEXT(D4)</f>
         <v>=AVERAGE(B2:B246)</v>
+      </c>
+      <c r="F4" s="15" t="n">
+        <f aca="false">AVERAGE(B2:B246)</f>
+        <v>3.75787755102041</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>